<commit_message>
Fix Excel export to exclude header in Save_Settings
- Updated the Save_Settings function in MSO5000_LCR.py to set header=False when saving to Settings_Custom.xlsx, ensuring the file is saved without column headers.

- Also updated Settings_Custom.xlsx accordingly.
</commit_message>
<xml_diff>
--- a/MSO5000 LCR/Settings_Custom.xlsx
+++ b/MSO5000 LCR/Settings_Custom.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,71 +422,23 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>0</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>0</v>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>0</v>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>0</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Rounded</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>0.5</v>
+      <c r="B1" t="n">
+        <v>2</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+    <row r="2">
+      <c r="A2" t="inlineStr">
         <is>
           <t>Time_Delay</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>1</v>
+      <c r="B2" t="n">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>